<commit_message>
Wort on gtx, tiny change
</commit_message>
<xml_diff>
--- a/doc/Transactions.xlsx
+++ b/doc/Transactions.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\gproj\jq\jSQLBox\doc\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="9780"/>
   </bookViews>
@@ -16,51 +21,49 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
-  <si>
-    <t>ctx.getConnection(ds)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>事务中</t>
   </si>
   <si>
-    <t>事务开</t>
-  </si>
-  <si>
-    <t>事务回</t>
-  </si>
-  <si>
-    <t>事务提</t>
-  </si>
-  <si>
-    <t>无事</t>
-  </si>
-  <si>
-    <t>startTx</t>
-  </si>
-  <si>
-    <t>commTx</t>
-  </si>
-  <si>
-    <t>rollbackTx</t>
-  </si>
-  <si>
     <t>ManualTx</t>
   </si>
   <si>
-    <t>ctx.releaseConnection(Connection,ds)</t>
-  </si>
-  <si>
     <t>初始化</t>
   </si>
   <si>
-    <t>new ManualTx(ds)</t>
+    <t>无事务</t>
+  </si>
+  <si>
+    <t>return ds.getConnection();</t>
+  </si>
+  <si>
+    <t>isInTransaction(ds)</t>
+  </si>
+  <si>
+    <t>releaseConnection(conn,ds)</t>
+  </si>
+  <si>
+    <t>getConnection(ds)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> if (conn != null)  
+            conn.close(); </t>
+  </si>
+  <si>
+    <t xml:space="preserve">事务开 beginTransaction() </t>
+  </si>
+  <si>
+    <t>事务滚 commit()</t>
+  </si>
+  <si>
+    <t>事务提 rollback()</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -78,7 +81,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -101,63 +104,20 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -165,77 +125,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -249,7 +144,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="F0F0F0"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -284,7 +179,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -317,9 +212,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -352,6 +264,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -528,112 +457,82 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:F2"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.42578125" customWidth="1"/>
-    <col min="3" max="3" width="8.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="25" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="4"/>
-      <c r="B3" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:F2"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Work on GTX, doc
</commit_message>
<xml_diff>
--- a/doc/Transactions.xlsx
+++ b/doc/Transactions.xlsx
@@ -1,19 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\gproj\jq\jSQLBox\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="9780"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="9780" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="ManualTx" sheetId="1" r:id="rId1"/>
+    <sheet name="TinyTx" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -21,53 +16,105 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
-  <si>
-    <t>事务中</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="24">
   <si>
     <t>ManualTx</t>
   </si>
   <si>
-    <t>初始化</t>
-  </si>
-  <si>
-    <t>无事务</t>
-  </si>
-  <si>
-    <t>return ds.getConnection();</t>
-  </si>
-  <si>
-    <t>isInTransaction(ds)</t>
-  </si>
-  <si>
-    <t>releaseConnection(conn,ds)</t>
-  </si>
-  <si>
-    <t>getConnection(ds)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> if (conn != null)  
-            conn.close(); </t>
-  </si>
-  <si>
-    <t xml:space="preserve">事务开 beginTransaction() </t>
-  </si>
-  <si>
-    <t>事务滚 commit()</t>
-  </si>
-  <si>
-    <t>事务提 rollback()</t>
+    <t>return connection!=null</t>
+  </si>
+  <si>
+    <t>事务未开启</t>
+  </si>
+  <si>
+    <t>事务已开启</t>
+  </si>
+  <si>
+    <t>如connection已存在，报错</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>如conn不为空，强制关掉它</t>
+  </si>
+  <si>
+    <t>如connection已存在，不做任何事</t>
+  </si>
+  <si>
+    <t>connection为空，从ds获取一个</t>
+  </si>
+  <si>
+    <t>connection已存在，直接返回保存的这个</t>
+  </si>
+  <si>
+    <t>从ds获取一个连接，并关闭自动提交</t>
+  </si>
+  <si>
+    <t>回滚connection,设为自动提交后清空</t>
+  </si>
+  <si>
+    <t>提交connection,设为自动提交后清空</t>
+  </si>
+  <si>
+    <t>检测事务 tx.isInTransaction(ds)</t>
+  </si>
+  <si>
+    <t>获取连接 tx.getConnection(ds)</t>
+  </si>
+  <si>
+    <t>释放连接 tx.releaseConnection(conn,ds)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">事务开启  tx.beginTransaction() </t>
+  </si>
+  <si>
+    <t>事务提交tx.rollback()</t>
+  </si>
+  <si>
+    <t>事务回滚  tx.commit()</t>
+  </si>
+  <si>
+    <t>特点：在ManualTx中保存一个Connection变量，作为事务已开启的凭证
+缺点：SqlBoxContext实例和ManualTx线程不安全，使用时每个线程都必须动态创建一个ManualTx和一个CTX：
+初始化:
+ManualTx tx=new ManualTx(ds);
+SqlBoxContext ctx=new SqlBoxContext(ds); 
+ctx.setConnectionManager(tx);</t>
+  </si>
+  <si>
+    <t>TinyTxConnectionManager</t>
+  </si>
+  <si>
+    <t>事务提交 tx.rollback()</t>
+  </si>
+  <si>
+    <t>事务回滚 tx.commit()</t>
+  </si>
+  <si>
+    <t>特点：在TinyTxConnectionManager中保存一个ThreadLocal Map变量，针对每个CTX的DS，检查它的DS是否已分配或绑定了connection
+优点：SqlBoxContext实例和DS可以只创建一个，通过ThreadLocal技术来实现多线程下自动切换Connection
+初始化:
+TinyTxConnectionManager tx=new TinyTxConnectionManager(ds);
+SqlBoxContext ctx=new SqlBoxContext(ds); 
+ctx.setConnectionManager(tx);</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -81,7 +128,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -104,20 +151,70 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -125,6 +222,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -144,7 +309,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="F0F0F0"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -179,7 +344,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -212,26 +377,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -264,23 +412,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -457,94 +588,229 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="25" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="38.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="41" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="1"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+      <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B4:C4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:C2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="38.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.42578125" style="7" customWidth="1"/>
+    <col min="3" max="3" width="53.5703125" style="7" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:3" ht="87.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="6"/>
+    </row>
+    <row r="5" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="B4:C4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Work on gtx, clean up old tx
</commit_message>
<xml_diff>
--- a/doc/Transactions.xlsx
+++ b/doc/Transactions.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18067"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\gproj\jq\jSQLBox\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="9780" activeTab="5"/>
+    <workbookView xWindow="480" yWindow="45" windowWidth="22995" windowHeight="9780" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="ManualTx" sheetId="1" r:id="rId1"/>
@@ -104,9 +99,6 @@
     <t>事务回滚  tx.commit(ds)</t>
   </si>
   <si>
-    <t xml:space="preserve">事务开启  tx.beginTransaction(ds,int) </t>
-  </si>
-  <si>
     <t>绑定在ds上的和传入的conn是同一个，不做任何事</t>
   </si>
   <si>
@@ -222,9 +214,6 @@
   </si>
   <si>
     <t>简单说，使用TinyTxConnectionManager只需要全局创建若干SqlBoxConext单例和TinyTxConnectionManager单例即可，事务的开启由TinyTxConnectionManager来决定，通常可以创建多个TinyTx切面，通过不同的自定义事务切面注解来开启不同的事务。</t>
-  </si>
-  <si>
-    <t>简单说，TinyTxConnectionManager每次只能针对一个DS开启事务，而GroupTxConnectionManager可以针对一组DS开启事务，但只能用于实际操作会收敛到单个数据库的场合，通常用于数据源由分库键决定，但不会同时操作多个数据源的分库分表场合，这种情况下不涉及分布式事务问题。</t>
   </si>
   <si>
     <t xml:space="preserve">特点：GtxConnectionManager是一个分布式事务工具，GtxConnectionManager初始化时内部保存一个ds数组，它通常设定为单例来使用。它通过一个ThreadLocal来管理传入的多个ds以及绑定在它上面的conn,当事务提交时，所有绑定在这组ds上的conn都会提交，它的事务判定是基于当前线程inGtxTransation threadlocal变量设定。
@@ -237,11 +226,17 @@
 ctx1.setConnectionManager(gm);
 ctx2.setConnectionManager(gm); </t>
   </si>
+  <si>
+    <t xml:space="preserve">事务开启  tx.startTransaction(ds,int) </t>
+  </si>
+  <si>
+    <t>简单说，TinyTxConnectionManager每次只能针对一个DS开启事务，而GroupTxConnectionManager可以针对一组DS开启事务， 通常用于实际操作会收敛到单个数据库的分库分表场合，这种情况下不涉及分布式事务问题。</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -366,11 +361,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -378,6 +373,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -397,7 +460,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="F0F0F0"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -432,7 +495,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -465,26 +528,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -517,23 +563,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -733,7 +762,7 @@
     </row>
     <row r="2" spans="1:3" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -814,11 +843,11 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="12" t="s">
-        <v>55</v>
-      </c>
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
+      <c r="A13" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -843,26 +872,26 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" s="6" customFormat="1" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
-        <v>36</v>
-      </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
+      <c r="A2" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
     </row>
     <row r="3" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="5" spans="1:3" ht="49.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
+      <c r="A5" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -877,8 +906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,7 +927,7 @@
     </row>
     <row r="2" spans="1:3" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -933,7 +962,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -947,13 +976,13 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -983,23 +1012,23 @@
         <v>16</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>58</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
+      <c r="A15" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1029,12 +1058,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1046,8 +1075,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1060,21 +1089,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" ht="138.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
@@ -1102,7 +1131,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1110,65 +1139,65 @@
         <v>12</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>28</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>38</v>
-      </c>
     </row>
     <row r="15" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="B15" s="12"/>
-      <c r="C15" s="12"/>
+      <c r="A15" s="11" t="s">
+        <v>60</v>
+      </c>
+      <c r="B15" s="11"/>
+      <c r="C15" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1184,8 +1213,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="85" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1197,21 +1226,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
     </row>
     <row r="2" spans="1:3" ht="177" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>2</v>
@@ -1239,7 +1268,7 @@
         <v>21</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1247,16 +1276,16 @@
         <v>12</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6" s="10"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>23</v>
@@ -1264,24 +1293,24 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1291,19 +1320,19 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C12" s="4"/>
     </row>

</xml_diff>